<commit_message>
Added Sprint 1 sample code
</commit_message>
<xml_diff>
--- a/User Stories/ASDE_Training_USER_STORIES.xlsx
+++ b/User Stories/ASDE_Training_USER_STORIES.xlsx
@@ -359,6 +359,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>The following classes of tests need to be implemented:-
 a)</t>
     </r>
@@ -612,6 +619,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">The following screens need to be developed:
 a) </t>
     </r>
@@ -863,10 +876,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -933,13 +946,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -949,7 +955,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -971,8 +977,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -993,9 +1007,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1011,7 +1025,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1024,15 +1045,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1042,14 +1054,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1083,13 +1096,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1101,37 +1138,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1155,7 +1174,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1167,97 +1258,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1268,15 +1281,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1334,17 +1338,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1360,11 +1360,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1373,15 +1386,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1394,131 +1407,131 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1535,9 +1548,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1894,8 +1904,8 @@
   <sheetPr/>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:L42"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A31" sqref="$A31:$XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1927,49 +1937,49 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" ht="18.75" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="14"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
@@ -2016,17 +2026,17 @@
       <c r="L7" s="5"/>
     </row>
     <row r="8" spans="2:2">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:2">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:2">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2067,17 +2077,17 @@
       <c r="L12" s="5"/>
     </row>
     <row r="13" spans="2:2">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:2">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:2">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2085,32 +2095,32 @@
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="2" t="s">
@@ -2178,32 +2188,32 @@
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
@@ -2253,45 +2263,45 @@
       <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="2"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
@@ -2377,45 +2387,45 @@
       <c r="A37" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" ht="20" customHeight="1" spans="1:11">
       <c r="A38" s="2"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="2" t="s">
@@ -2447,18 +2457,18 @@
       <c r="A42" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -2525,35 +2535,35 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" ht="18.75" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
@@ -2656,32 +2666,32 @@
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
@@ -2765,15 +2775,15 @@
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="2" t="s">
@@ -2805,45 +2815,45 @@
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="2"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
@@ -2875,18 +2885,18 @@
       <c r="A27" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2947,35 +2957,35 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" ht="18.75" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
@@ -3060,18 +3070,18 @@
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
@@ -3101,53 +3111,53 @@
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" ht="18" customHeight="1" spans="1:12">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
@@ -3249,46 +3259,46 @@
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="2"/>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="2"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="2" t="s">
@@ -3334,45 +3344,45 @@
       <c r="A29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="2"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="2" t="s">
@@ -3404,32 +3414,32 @@
       <c r="A34" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
@@ -3461,18 +3471,18 @@
       <c r="A39" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -3544,35 +3554,35 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" ht="18.75" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
@@ -3639,7 +3649,7 @@
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>86</v>
       </c>
       <c r="C8" s="5"/>
@@ -3657,18 +3667,18 @@
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
@@ -3698,43 +3708,43 @@
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" ht="99" customHeight="1" spans="1:12">
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>91</v>
       </c>
       <c r="C15" s="4"/>
@@ -3752,7 +3762,7 @@
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="11" t="s">
         <v>92</v>
       </c>
       <c r="C16" s="4"/>
@@ -3770,7 +3780,7 @@
       <c r="A17" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="11" t="s">
         <v>94</v>
       </c>
       <c r="C17" s="4"/>
@@ -3788,7 +3798,7 @@
       <c r="A18" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="11" t="s">
         <v>96</v>
       </c>
       <c r="C18" s="4"/>
@@ -3806,7 +3816,7 @@
       <c r="A19" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="11" t="s">
         <v>98</v>
       </c>
       <c r="C19" s="4"/>
@@ -3824,7 +3834,7 @@
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="11" t="s">
         <v>99</v>
       </c>
       <c r="C20" s="4"/>
@@ -3936,7 +3946,7 @@
       <c r="A28" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="11" t="s">
         <v>96</v>
       </c>
       <c r="C28" s="4"/>
@@ -3954,7 +3964,7 @@
       <c r="A29" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="11" t="s">
         <v>98</v>
       </c>
       <c r="C29" s="4"/>
@@ -3972,31 +3982,31 @@
       <c r="A30" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="2"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
@@ -4096,31 +4106,31 @@
       <c r="A38" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="2"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="2" t="s">
@@ -4166,32 +4176,32 @@
       <c r="A43" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="8"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="B45" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="2" t="s">
@@ -4223,18 +4233,18 @@
       <c r="A48" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="35">
@@ -4330,22 +4340,22 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" ht="18.75" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
@@ -4409,36 +4419,36 @@
       <c r="L7" s="5"/>
     </row>
     <row r="8" ht="17" customHeight="1" spans="1:12">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
     </row>
     <row r="9" ht="103" customHeight="1" spans="1:12">
-      <c r="A9" s="6"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="2" t="s">
@@ -4606,18 +4616,18 @@
       <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
@@ -4647,37 +4657,37 @@
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="2" t="s">
@@ -4701,7 +4711,7 @@
       <c r="A26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="10" t="s">
         <v>135</v>
       </c>
     </row>
@@ -4709,7 +4719,7 @@
       <c r="A27" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B27" s="11" t="s">
         <v>136</v>
       </c>
       <c r="C27" s="4"/>
@@ -4759,17 +4769,17 @@
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="2" t="s">
@@ -4855,7 +4865,7 @@
       <c r="A36" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="11" t="s">
         <v>143</v>
       </c>
       <c r="C36" s="4"/>
@@ -4873,7 +4883,7 @@
       <c r="A37" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="11" t="s">
         <v>144</v>
       </c>
       <c r="C37" s="4"/>
@@ -4891,31 +4901,31 @@
       <c r="A38" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="2"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="2" t="s">
@@ -4979,32 +4989,32 @@
       <c r="A44" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B46" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="2" t="s">
@@ -5036,18 +5046,18 @@
       <c r="A49" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="9"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="38">

</xml_diff>

<commit_message>
Added Spring Data materials
</commit_message>
<xml_diff>
--- a/User Stories/ASDE_Training_USER_STORIES.xlsx
+++ b/User Stories/ASDE_Training_USER_STORIES.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="2" r:id="rId1"/>
@@ -876,10 +876,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -924,6 +924,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -939,23 +946,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -977,23 +970,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1007,9 +985,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1031,8 +1009,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1040,13 +1033,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1062,7 +1048,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1081,7 +1081,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1090,13 +1090,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,43 +1108,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1162,7 +1138,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1174,7 +1150,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1186,25 +1174,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1222,7 +1234,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1234,31 +1264,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1270,7 +1276,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1323,6 +1329,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1334,6 +1349,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1352,32 +1382,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1386,7 +1392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1404,134 +1410,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1574,10 +1580,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1904,7 +1931,7 @@
   <sheetPr/>
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="A31" sqref="$A31:$XFD37"/>
     </sheetView>
   </sheetViews>
@@ -2026,17 +2053,17 @@
       <c r="L7" s="5"/>
     </row>
     <row r="8" spans="2:2">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="23" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:2">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:2">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="23" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2077,17 +2104,17 @@
       <c r="L12" s="5"/>
     </row>
     <row r="13" spans="2:2">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="23" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:2">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:2">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="23" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3521,8 +3548,8 @@
   <sheetPr/>
   <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A45" sqref="$A45:$XFD48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29:L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3584,101 +3611,113 @@
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:12">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="16"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="16" t="s">
         <v>8</v>
       </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
     </row>
     <row r="6" ht="20" customHeight="1" spans="1:12">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="16"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="2" t="s">
@@ -3726,7 +3765,7 @@
       <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="21" t="s">
         <v>90</v>
       </c>
       <c r="C14" s="9"/>
@@ -3741,22 +3780,22 @@
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="2" t="s">

</xml_diff>